<commit_message>
Solution based out of feature engineering and CNN
</commit_message>
<xml_diff>
--- a/Titanic Survival Prediction/output_logistic_regression.xlsx
+++ b/Titanic Survival Prediction/output_logistic_regression.xlsx
@@ -420,7 +420,7 @@
         <v>895</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -444,7 +444,7 @@
         <v>898</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -532,7 +532,7 @@
         <v>909</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -612,7 +612,7 @@
         <v>919</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -660,7 +660,7 @@
         <v>925</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -676,7 +676,7 @@
         <v>927</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -684,7 +684,7 @@
         <v>928</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -692,7 +692,7 @@
         <v>929</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -788,7 +788,7 @@
         <v>941</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -908,7 +908,7 @@
         <v>956</v>
       </c>
       <c r="B66">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -924,7 +924,7 @@
         <v>958</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -996,7 +996,7 @@
         <v>967</v>
       </c>
       <c r="B77">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1036,7 +1036,7 @@
         <v>972</v>
       </c>
       <c r="B82">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1092,7 +1092,7 @@
         <v>979</v>
       </c>
       <c r="B89">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1100,7 +1100,7 @@
         <v>980</v>
       </c>
       <c r="B90">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1180,7 +1180,7 @@
         <v>990</v>
       </c>
       <c r="B100">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1284,7 +1284,7 @@
         <v>1003</v>
       </c>
       <c r="B113">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1300,7 +1300,7 @@
         <v>1005</v>
       </c>
       <c r="B115">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1452,7 +1452,7 @@
         <v>1024</v>
       </c>
       <c r="B134">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -1500,7 +1500,7 @@
         <v>1030</v>
       </c>
       <c r="B140">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -1532,7 +1532,7 @@
         <v>1034</v>
       </c>
       <c r="B144">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -1548,7 +1548,7 @@
         <v>1036</v>
       </c>
       <c r="B146">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -1652,7 +1652,7 @@
         <v>1049</v>
       </c>
       <c r="B159">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -1660,7 +1660,7 @@
         <v>1050</v>
       </c>
       <c r="B160">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -1668,7 +1668,7 @@
         <v>1051</v>
       </c>
       <c r="B161">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -1676,7 +1676,7 @@
         <v>1052</v>
       </c>
       <c r="B162">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -1684,7 +1684,7 @@
         <v>1053</v>
       </c>
       <c r="B163">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -1748,7 +1748,7 @@
         <v>1061</v>
       </c>
       <c r="B171">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -1964,7 +1964,7 @@
         <v>1088</v>
       </c>
       <c r="B198">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -1972,7 +1972,7 @@
         <v>1089</v>
       </c>
       <c r="B199">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -1988,7 +1988,7 @@
         <v>1091</v>
       </c>
       <c r="B201">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -2012,7 +2012,7 @@
         <v>1094</v>
       </c>
       <c r="B204">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -2100,7 +2100,7 @@
         <v>1105</v>
       </c>
       <c r="B215">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -2108,7 +2108,7 @@
         <v>1106</v>
       </c>
       <c r="B216">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="217" spans="1:2">
@@ -2132,7 +2132,7 @@
         <v>1109</v>
       </c>
       <c r="B219">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="220" spans="1:2">
@@ -2180,7 +2180,7 @@
         <v>1115</v>
       </c>
       <c r="B225">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="226" spans="1:2">
@@ -2196,7 +2196,7 @@
         <v>1117</v>
       </c>
       <c r="B227">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="228" spans="1:2">
@@ -2212,7 +2212,7 @@
         <v>1119</v>
       </c>
       <c r="B229">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="230" spans="1:2">
@@ -2284,7 +2284,7 @@
         <v>1128</v>
       </c>
       <c r="B238">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="239" spans="1:2">
@@ -2292,7 +2292,7 @@
         <v>1129</v>
       </c>
       <c r="B239">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="240" spans="1:2">
@@ -2388,7 +2388,7 @@
         <v>1141</v>
       </c>
       <c r="B251">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="252" spans="1:2">
@@ -2412,7 +2412,7 @@
         <v>1144</v>
       </c>
       <c r="B254">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="255" spans="1:2">
@@ -2460,7 +2460,7 @@
         <v>1150</v>
       </c>
       <c r="B260">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="261" spans="1:2">
@@ -2540,7 +2540,7 @@
         <v>1160</v>
       </c>
       <c r="B270">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="271" spans="1:2">
@@ -2636,7 +2636,7 @@
         <v>1172</v>
       </c>
       <c r="B282">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="283" spans="1:2">
@@ -2652,7 +2652,7 @@
         <v>1174</v>
       </c>
       <c r="B284">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="285" spans="1:2">
@@ -2660,7 +2660,7 @@
         <v>1175</v>
       </c>
       <c r="B285">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="286" spans="1:2">
@@ -2668,7 +2668,7 @@
         <v>1176</v>
       </c>
       <c r="B286">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="287" spans="1:2">
@@ -2724,7 +2724,7 @@
         <v>1183</v>
       </c>
       <c r="B293">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="294" spans="1:2">
@@ -2740,7 +2740,7 @@
         <v>1185</v>
       </c>
       <c r="B295">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="296" spans="1:2">
@@ -2828,7 +2828,7 @@
         <v>1196</v>
       </c>
       <c r="B306">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="307" spans="1:2">
@@ -2884,7 +2884,7 @@
         <v>1203</v>
       </c>
       <c r="B313">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="314" spans="1:2">
@@ -2924,7 +2924,7 @@
         <v>1208</v>
       </c>
       <c r="B318">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="319" spans="1:2">
@@ -2932,7 +2932,7 @@
         <v>1209</v>
       </c>
       <c r="B319">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="320" spans="1:2">
@@ -3300,7 +3300,7 @@
         <v>1255</v>
       </c>
       <c r="B365">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="366" spans="1:2">
@@ -3332,7 +3332,7 @@
         <v>1259</v>
       </c>
       <c r="B369">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="370" spans="1:2">
@@ -3348,7 +3348,7 @@
         <v>1261</v>
       </c>
       <c r="B371">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="372" spans="1:2">
@@ -3404,7 +3404,7 @@
         <v>1268</v>
       </c>
       <c r="B378">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="379" spans="1:2">
@@ -3460,7 +3460,7 @@
         <v>1275</v>
       </c>
       <c r="B385">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="386" spans="1:2">
@@ -3516,7 +3516,7 @@
         <v>1282</v>
       </c>
       <c r="B392">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="393" spans="1:2">
@@ -3620,7 +3620,7 @@
         <v>1295</v>
       </c>
       <c r="B405">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="406" spans="1:2">
@@ -3652,7 +3652,7 @@
         <v>1299</v>
       </c>
       <c r="B409">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="410" spans="1:2">
@@ -3660,7 +3660,7 @@
         <v>1300</v>
       </c>
       <c r="B410">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="411" spans="1:2">
@@ -3668,7 +3668,7 @@
         <v>1301</v>
       </c>
       <c r="B411">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="412" spans="1:2">
@@ -3676,7 +3676,7 @@
         <v>1302</v>
       </c>
       <c r="B412">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="413" spans="1:2">

</xml_diff>